<commit_message>
fixed Structure Scheduler misbehaviour
</commit_message>
<xml_diff>
--- a/fesch/output/log_001.xlsx
+++ b/fesch/output/log_001.xlsx
@@ -35,40 +35,40 @@
     <t>Dr. Csorba Kristóf</t>
   </si>
   <si>
+    <t>Dr. Balogh Attila</t>
+  </si>
+  <si>
+    <t>Dr. Kovács Tibor</t>
+  </si>
+  <si>
+    <t>Dr. Kővári Bence András</t>
+  </si>
+  <si>
+    <t>Dr. Forstner Bertalan</t>
+  </si>
+  <si>
+    <t>Dr. Varjasi István</t>
+  </si>
+  <si>
+    <t>Dr. Mezei Gergely</t>
+  </si>
+  <si>
+    <t>Secretary</t>
+  </si>
+  <si>
+    <t>Kovács Adorján</t>
+  </si>
+  <si>
+    <t>Erdős Szilvia</t>
+  </si>
+  <si>
+    <t>Somogyi Norbert Zsolt</t>
+  </si>
+  <si>
+    <t>Pásztor Dániel</t>
+  </si>
+  <si>
     <t>Sik Tamás Dávid</t>
-  </si>
-  <si>
-    <t>Dr. Kovács Tibor</t>
-  </si>
-  <si>
-    <t>Dr. Kővári Bence András</t>
-  </si>
-  <si>
-    <t>Dr. Forstner Bertalan</t>
-  </si>
-  <si>
-    <t>Dr. Varjasi István</t>
-  </si>
-  <si>
-    <t>Dr. Mezei Gergely</t>
-  </si>
-  <si>
-    <t>Secretary</t>
-  </si>
-  <si>
-    <t>Kovács Adorján</t>
-  </si>
-  <si>
-    <t>Erdős Szilvia</t>
-  </si>
-  <si>
-    <t>Somogyi Norbert Zsolt</t>
-  </si>
-  <si>
-    <t>Pásztor Dániel</t>
-  </si>
-  <si>
-    <t>Dr. Balogh Attila</t>
   </si>
   <si>
     <t>Pomázi Krisztián Dániel</t>

</xml_diff>